<commit_message>
Add Project6 EF Core Warung Makan Bahari
</commit_message>
<xml_diff>
--- a/Project5_SQL/WarungMakanBahari.xlsx
+++ b/Project5_SQL/WarungMakanBahari.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\source\ProjectEnigmaCamp\Project5_SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AD1686-B29F-4893-B140-6115B501298F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473AD40C-A717-4EB6-8069-213B384A75FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{4F8FBA49-CC45-4E2E-92C1-B572A047B8FD}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1NF'!$B$4:$L$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2NF'!$F$3:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2NF'!$E$3:$H$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UNF!$B$5:$J$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="199">
   <si>
     <t>Data Nota Juni 2022</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
     <t>CUS01</t>
   </si>
   <si>
@@ -547,6 +544,99 @@
   </si>
   <si>
     <t>Total Transaction After Dsc</t>
+  </si>
+  <si>
+    <t>Price_Table</t>
+  </si>
+  <si>
+    <t>Price_Id PK</t>
+  </si>
+  <si>
+    <t>PR01</t>
+  </si>
+  <si>
+    <t>PR02</t>
+  </si>
+  <si>
+    <t>PR03</t>
+  </si>
+  <si>
+    <t>PR04</t>
+  </si>
+  <si>
+    <t>PR05</t>
+  </si>
+  <si>
+    <t>PR06</t>
+  </si>
+  <si>
+    <t>PR07</t>
+  </si>
+  <si>
+    <t>PR08</t>
+  </si>
+  <si>
+    <t>PR09</t>
+  </si>
+  <si>
+    <t>PR10</t>
+  </si>
+  <si>
+    <t>PR11</t>
+  </si>
+  <si>
+    <t>PR12</t>
+  </si>
+  <si>
+    <t>PR13</t>
+  </si>
+  <si>
+    <t>PR14</t>
+  </si>
+  <si>
+    <t>PR15</t>
+  </si>
+  <si>
+    <t>PR16</t>
+  </si>
+  <si>
+    <t>PR17</t>
+  </si>
+  <si>
+    <t>PR18</t>
+  </si>
+  <si>
+    <t>PR19</t>
+  </si>
+  <si>
+    <t>PR20</t>
+  </si>
+  <si>
+    <t>PR21</t>
+  </si>
+  <si>
+    <t>PR22</t>
+  </si>
+  <si>
+    <t>Meja_Table</t>
+  </si>
+  <si>
+    <t>Meja_Id PK</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>ots</t>
+  </si>
+  <si>
+    <t>tk</t>
+  </si>
+  <si>
+    <t>Price_Id FK</t>
   </si>
 </sst>
 </file>
@@ -557,7 +647,7 @@
     <numFmt numFmtId="42" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;Rp&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +702,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -633,7 +729,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -765,15 +861,43 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -850,7 +974,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -858,24 +981,53 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2922,1072 +3074,1290 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3A3836-B6E8-481B-BFE1-0C6DFAB6347A}">
-  <dimension ref="B2:O38"/>
+  <dimension ref="B2:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" customWidth="1"/>
-    <col min="7" max="7" width="17.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" customWidth="1"/>
-    <col min="10" max="10" width="21.6328125" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" customWidth="1"/>
-    <col min="14" max="14" width="11.26953125" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="21.6328125" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="18.6328125" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="F2" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="L2" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="K2" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N4" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="23">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="K13" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="F14" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="G14" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="O3" s="6" t="s">
+      <c r="K14" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="20">
-        <v>2000</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="F15" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="33">
+        <v>10500</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="23">
-        <v>0</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O4" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="20">
-        <v>6000</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="33">
+        <v>11000</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="N16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="23">
-        <v>0</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="33">
+        <v>15300</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N17" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="s">
+      <c r="C18" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I18" s="33">
+        <v>25000</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M18" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="20">
-        <v>1500</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="23">
-        <v>1</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="M6" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" s="9" t="s">
+      <c r="N18" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="33">
+        <v>11000</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="O6" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="20">
-        <v>1500</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="23">
-        <v>0</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="M7" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O7" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="20">
-        <v>10000</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="23">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O8" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="20">
-        <v>10000</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="23">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="O9" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="20">
-        <v>4000</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="23">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="20">
-        <v>12000</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="23">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="20">
-        <v>25000</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="O12" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="20">
-        <v>3000</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="L13" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="O13" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="20">
-        <v>3000</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="O14" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="20">
-        <v>1500</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="38">
-        <v>10500</v>
-      </c>
-      <c r="L15" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="M15" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O15" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="20">
-        <v>2500</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="38">
-        <v>11000</v>
-      </c>
-      <c r="L16" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="M16" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="O16" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="20">
-        <v>2000</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="38">
-        <v>15300</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="M17" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="O17" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="20">
-        <v>3000</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" s="38">
-        <v>25000</v>
-      </c>
-      <c r="L18" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O18" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="20">
-        <v>2000</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="38">
-        <v>11000</v>
-      </c>
-      <c r="L19" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="O19" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="20">
-        <v>4000</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>83</v>
+      <c r="E20" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="38">
+      <c r="I20" s="33">
         <v>14000</v>
       </c>
+      <c r="K20" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="L20" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="N20" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O20" s="22">
+        <v>114</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N20" s="22">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="20">
-        <v>5000</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>84</v>
+      <c r="E21" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="38">
+      <c r="I21" s="33">
         <v>14400</v>
       </c>
-      <c r="L21" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="M21" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="O21" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K21" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="20">
-        <v>5000</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>85</v>
+      <c r="E22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="38">
+      <c r="I22" s="33">
         <v>14000</v>
       </c>
-      <c r="L22" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="M22" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="O22" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K22" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="N22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="20">
-        <v>2000</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>86</v>
+      <c r="E23" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="38">
+      <c r="I23" s="33">
         <v>10500</v>
       </c>
+      <c r="K23" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="L23" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O23" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N23" s="22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="20">
+      <c r="E24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="33">
+        <v>10000</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E25" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="33">
+        <v>11500</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="N25" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E26" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I26" s="33">
+        <v>30000</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N26" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K27" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K28" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N28" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B29" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="F29" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="G29" s="34"/>
+      <c r="K29" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="N29" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B30" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N30" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="20">
+        <v>2000</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="L31" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N31" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B32" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="20">
+        <v>6000</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="N32" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="20">
+        <v>1500</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="N33" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B34" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="20">
+        <v>1500</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N34" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B35" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="20">
+        <v>10000</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G35" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N35" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B36" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="20">
+        <v>10000</v>
+      </c>
+      <c r="K36" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N36" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B37" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="20">
+        <v>4000</v>
+      </c>
+      <c r="K37" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="L37" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="M37" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N37" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B38" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="20">
+        <v>12000</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N38" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B39" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="20">
+        <v>25000</v>
+      </c>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="40"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B40" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="20">
         <v>3000</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="38">
-        <v>10000</v>
-      </c>
-      <c r="L24" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N24" s="9" t="s">
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B41" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="20">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B42" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="20">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="20">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B44" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="20">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B45" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="20">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B47" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B48" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="20">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="O24" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="F25" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="38">
-        <v>11500</v>
-      </c>
-      <c r="L25" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="O25" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="F26" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="38">
-        <v>30000</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N26" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O26" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L27" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="N27" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="O27" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L28" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="M28" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O28" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L29" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="M29" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="N29" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="O29" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L30" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="M30" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="N30" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="O30" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L31" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="M31" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O31" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="L32" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="M32" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O32" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L33" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="O33" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L34" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="M34" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="N34" s="9" t="s">
+      <c r="D49" s="20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="20">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="O34" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L35" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="N35" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="O35" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L36" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="M36" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="O36" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L37" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="M37" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="N37" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="O37" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="12:15" x14ac:dyDescent="0.35">
-      <c r="L38" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O38" s="22">
-        <v>15</v>
+      <c r="D52" s="20">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="F13:J13"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:G29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="I4 I5:I7 I8:I11" numberStoredAsText="1"/>
+    <ignoredError sqref="H4 H5:H7 H8:H11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>